<commit_message>
Update Chaz Lanier Data
</commit_message>
<xml_diff>
--- a/Assignments/college_player_data.xlsx
+++ b/Assignments/college_player_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiocanete/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thejjserg/Documents/GitHub/basketball-analytics/Assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCF76C4B-E1F0-EE4C-A8AC-BD29BC536512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1BAD0E-176E-5341-A671-A4532481141B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="600" windowWidth="28040" windowHeight="16120" xr2:uid="{148BE54A-ED5D-384B-82BB-04AE40AA4B05}"/>
+    <workbookView xWindow="360" yWindow="680" windowWidth="28040" windowHeight="16120" xr2:uid="{148BE54A-ED5D-384B-82BB-04AE40AA4B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Chaz Lanier" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Season</t>
   </si>
@@ -210,6 +210,12 @@
       </rPr>
       <t>W-AA-1</t>
     </r>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Chaz Lanier</t>
   </si>
 </sst>
 </file>
@@ -641,625 +647,643 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDFDC7F-C622-3244-BDB3-6DEA5A66C85A}">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>10</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>0.6</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>1.6</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>0.375</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>0.3</v>
       </c>
-      <c r="M2" s="3">
+      <c r="N2" s="3">
         <v>1</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.3</v>
       </c>
       <c r="O2" s="3">
         <v>0.3</v>
       </c>
       <c r="P2" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="Q2" s="3">
         <v>0.6</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="R2" s="3">
         <v>0.5</v>
       </c>
-      <c r="R2" s="3">
+      <c r="S2" s="3">
         <v>0.46899999999999997</v>
       </c>
-      <c r="S2" s="3">
+      <c r="T2" s="3">
         <v>0.2</v>
       </c>
-      <c r="T2" s="3">
+      <c r="U2" s="3">
         <v>0.3</v>
       </c>
-      <c r="U2" s="3">
+      <c r="V2" s="3">
         <v>0.66700000000000004</v>
       </c>
-      <c r="V2" s="3">
+      <c r="W2" s="3">
         <v>0</v>
-      </c>
-      <c r="W2" s="3">
-        <v>0.7</v>
       </c>
       <c r="X2" s="3">
         <v>0.7</v>
       </c>
       <c r="Y2" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="Z2" s="3">
         <v>0.6</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="AA2" s="3">
         <v>0.3</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AB2" s="3">
         <v>0</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AC2" s="3">
         <v>0.3</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AD2" s="3">
         <v>0.4</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AE2" s="3">
         <v>1.7</v>
       </c>
-      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>31</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>8</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>21</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>1.4</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>3.4</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>0.41499999999999998</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>0.5</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>1.8</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>0.30399999999999999</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <v>0.9</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>1.6</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="3">
         <v>0.54</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="3">
         <v>0.495</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="3">
         <v>1.3</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="3">
         <v>0.80500000000000005</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="3">
         <v>0.8</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="3">
         <v>1.9</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="3">
         <v>2.7</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>0.7</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="3">
         <v>0.2</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="3">
         <v>0.5</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="3">
         <v>1</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="3">
         <v>4.5</v>
       </c>
-      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>31</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>9</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>19.7</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>1.7</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>3.8</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>0.45400000000000001</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>0.9</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>0.39100000000000001</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>0.9</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="3">
         <v>1.6</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="R4" s="3">
         <v>0.54</v>
       </c>
-      <c r="R4" s="3">
+      <c r="S4" s="3">
         <v>0.56699999999999995</v>
-      </c>
-      <c r="S4" s="3">
-        <v>0.3</v>
       </c>
       <c r="T4" s="3">
         <v>0.3</v>
       </c>
       <c r="U4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="V4" s="3">
         <v>1</v>
       </c>
-      <c r="V4" s="3">
+      <c r="W4" s="3">
         <v>0.5</v>
       </c>
-      <c r="W4" s="3">
+      <c r="X4" s="3">
         <v>2</v>
       </c>
-      <c r="X4" s="3">
+      <c r="Y4" s="3">
         <v>2.5</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Z4" s="3">
         <v>0.9</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="AA4" s="3">
         <v>0.4</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AB4" s="3">
         <v>0.2</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AC4" s="3">
         <v>0.5</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AD4" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AE4" s="3">
         <v>4.7</v>
       </c>
-      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>32</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>31</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>33.4</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>6.7</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>13.1</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>0.51</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>3.3</v>
       </c>
-      <c r="M5" s="3">
+      <c r="N5" s="3">
         <v>7.5</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <v>0.44</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="3">
         <v>3.4</v>
       </c>
-      <c r="P5" s="3">
+      <c r="Q5" s="3">
         <v>5.6</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="R5" s="3">
         <v>0.60299999999999998</v>
       </c>
-      <c r="R5" s="3">
+      <c r="S5" s="3">
         <v>0.63600000000000001</v>
       </c>
-      <c r="S5" s="3">
+      <c r="T5" s="3">
         <v>3</v>
       </c>
-      <c r="T5" s="3">
+      <c r="U5" s="3">
         <v>3.4</v>
       </c>
-      <c r="U5" s="3">
+      <c r="V5" s="3">
         <v>0.88</v>
       </c>
-      <c r="V5" s="3">
+      <c r="W5" s="3">
         <v>0.7</v>
       </c>
-      <c r="W5" s="3">
+      <c r="X5" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="X5" s="3">
+      <c r="Y5" s="3">
         <v>4.8</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Z5" s="3">
         <v>1.8</v>
       </c>
-      <c r="Z5" s="3">
+      <c r="AA5" s="3">
         <v>0.9</v>
       </c>
-      <c r="AA5" s="3">
+      <c r="AB5" s="3">
         <v>0.3</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AC5" s="3">
         <v>1.6</v>
       </c>
-      <c r="AC5" s="3">
+      <c r="AD5" s="3">
         <v>1.5</v>
       </c>
-      <c r="AD5" s="3">
+      <c r="AE5" s="3">
         <v>19.7</v>
       </c>
-      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F6" s="3">
-        <v>38</v>
       </c>
       <c r="G6" s="3">
         <v>38</v>
       </c>
       <c r="H6" s="3">
+        <v>38</v>
+      </c>
+      <c r="I6" s="3">
         <v>31.4</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>6.4</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>14.8</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>0.43099999999999999</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <v>3.2</v>
       </c>
-      <c r="M6" s="3">
+      <c r="N6" s="3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <v>0.39500000000000002</v>
       </c>
-      <c r="O6" s="3">
+      <c r="P6" s="3">
         <v>3.2</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <v>6.7</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <v>0.47399999999999998</v>
       </c>
-      <c r="R6" s="3">
+      <c r="S6" s="3">
         <v>0.54</v>
       </c>
-      <c r="S6" s="3">
+      <c r="T6" s="3">
         <v>2</v>
       </c>
-      <c r="T6" s="3">
+      <c r="U6" s="3">
         <v>2.6</v>
       </c>
-      <c r="U6" s="3">
+      <c r="V6" s="3">
         <v>0.75800000000000001</v>
       </c>
-      <c r="V6" s="3">
+      <c r="W6" s="3">
         <v>0.5</v>
       </c>
-      <c r="W6" s="3">
+      <c r="X6" s="3">
         <v>3.4</v>
       </c>
-      <c r="X6" s="3">
+      <c r="Y6" s="3">
         <v>3.9</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Z6" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Z6" s="3">
+      <c r="AA6" s="3">
         <v>0.9</v>
       </c>
-      <c r="AA6" s="3">
+      <c r="AB6" s="3">
         <v>0.1</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AC6" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AC6" s="3">
+      <c r="AD6" s="3">
         <v>1.6</v>
       </c>
-      <c r="AD6" s="3">
+      <c r="AE6" s="3">
         <v>18</v>
       </c>
-      <c r="AE6" s="5" t="s">
+      <c r="AF6" s="5" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2021" xr:uid="{C2259446-CE80-8949-BDB7-5C38ADDC30B9}"/>
-    <hyperlink ref="B2" r:id="rId2" display="https://www.sports-reference.com/cbb/schools/north-florida/men/2021.html" xr:uid="{E812B178-7B07-8644-BE95-D0EA95EC2814}"/>
-    <hyperlink ref="C2" r:id="rId3" display="https://www.sports-reference.com/cbb/conferences/atlantic-sun/men/2021.html" xr:uid="{05421C5A-8758-0441-8A0C-30153E5CAED4}"/>
-    <hyperlink ref="A3" r:id="rId4" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2022" xr:uid="{C2E4BE31-68B7-D846-9EF9-AE9DEF94C989}"/>
-    <hyperlink ref="B3" r:id="rId5" display="https://www.sports-reference.com/cbb/schools/north-florida/men/2022.html" xr:uid="{5D4E23BE-6075-834D-A5A1-28E5B29947E4}"/>
-    <hyperlink ref="C3" r:id="rId6" display="https://www.sports-reference.com/cbb/conferences/atlantic-sun/men/2022.html" xr:uid="{30839EE4-68EF-1645-A8AD-A6BD2555B879}"/>
-    <hyperlink ref="A4" r:id="rId7" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2023" xr:uid="{4E8CF452-FEF9-E846-BC8A-1C6B53550FD8}"/>
-    <hyperlink ref="B4" r:id="rId8" display="https://www.sports-reference.com/cbb/schools/north-florida/men/2023.html" xr:uid="{9582569A-3704-5A41-83AF-372FD4C247DF}"/>
-    <hyperlink ref="C4" r:id="rId9" display="https://www.sports-reference.com/cbb/conferences/atlantic-sun/men/2023.html" xr:uid="{5AF24EF9-586A-2F43-9FAD-1CC89E2E527E}"/>
-    <hyperlink ref="A5" r:id="rId10" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2024" xr:uid="{04EFB852-B38D-D44B-87A5-94EE863CD16F}"/>
-    <hyperlink ref="B5" r:id="rId11" display="https://www.sports-reference.com/cbb/schools/north-florida/men/2024.html" xr:uid="{015E831B-D3BC-0F4E-9EE6-6C6D0A03AB2F}"/>
-    <hyperlink ref="C5" r:id="rId12" display="https://www.sports-reference.com/cbb/conferences/atlantic-sun/men/2024.html" xr:uid="{299874B2-44BE-5247-AC33-4F85F3D9ACFF}"/>
-    <hyperlink ref="A6" r:id="rId13" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2025" xr:uid="{1C705188-85AE-8C44-8C34-5F576B687717}"/>
-    <hyperlink ref="B6" r:id="rId14" display="https://www.sports-reference.com/cbb/schools/tennessee/men/2025.html" xr:uid="{6FA85B33-BA8C-DF4D-A676-206EEB1FA73E}"/>
-    <hyperlink ref="C6" r:id="rId15" display="https://www.sports-reference.com/cbb/conferences/sec/men/2025.html" xr:uid="{7F9088DD-188F-344A-951A-306A0AC08E48}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2021" xr:uid="{C2259446-CE80-8949-BDB7-5C38ADDC30B9}"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://www.sports-reference.com/cbb/schools/north-florida/men/2021.html" xr:uid="{E812B178-7B07-8644-BE95-D0EA95EC2814}"/>
+    <hyperlink ref="D2" r:id="rId3" display="https://www.sports-reference.com/cbb/conferences/atlantic-sun/men/2021.html" xr:uid="{05421C5A-8758-0441-8A0C-30153E5CAED4}"/>
+    <hyperlink ref="B3" r:id="rId4" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2022" xr:uid="{C2E4BE31-68B7-D846-9EF9-AE9DEF94C989}"/>
+    <hyperlink ref="C3" r:id="rId5" display="https://www.sports-reference.com/cbb/schools/north-florida/men/2022.html" xr:uid="{5D4E23BE-6075-834D-A5A1-28E5B29947E4}"/>
+    <hyperlink ref="D3" r:id="rId6" display="https://www.sports-reference.com/cbb/conferences/atlantic-sun/men/2022.html" xr:uid="{30839EE4-68EF-1645-A8AD-A6BD2555B879}"/>
+    <hyperlink ref="B4" r:id="rId7" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2023" xr:uid="{4E8CF452-FEF9-E846-BC8A-1C6B53550FD8}"/>
+    <hyperlink ref="C4" r:id="rId8" display="https://www.sports-reference.com/cbb/schools/north-florida/men/2023.html" xr:uid="{9582569A-3704-5A41-83AF-372FD4C247DF}"/>
+    <hyperlink ref="D4" r:id="rId9" display="https://www.sports-reference.com/cbb/conferences/atlantic-sun/men/2023.html" xr:uid="{5AF24EF9-586A-2F43-9FAD-1CC89E2E527E}"/>
+    <hyperlink ref="B5" r:id="rId10" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2024" xr:uid="{04EFB852-B38D-D44B-87A5-94EE863CD16F}"/>
+    <hyperlink ref="C5" r:id="rId11" display="https://www.sports-reference.com/cbb/schools/north-florida/men/2024.html" xr:uid="{015E831B-D3BC-0F4E-9EE6-6C6D0A03AB2F}"/>
+    <hyperlink ref="D5" r:id="rId12" display="https://www.sports-reference.com/cbb/conferences/atlantic-sun/men/2024.html" xr:uid="{299874B2-44BE-5247-AC33-4F85F3D9ACFF}"/>
+    <hyperlink ref="B6" r:id="rId13" display="https://www.sports-reference.com/cbb/players/chaz-lanier-1/gamelog/2025" xr:uid="{1C705188-85AE-8C44-8C34-5F576B687717}"/>
+    <hyperlink ref="C6" r:id="rId14" display="https://www.sports-reference.com/cbb/schools/tennessee/men/2025.html" xr:uid="{6FA85B33-BA8C-DF4D-A676-206EEB1FA73E}"/>
+    <hyperlink ref="D6" r:id="rId15" display="https://www.sports-reference.com/cbb/conferences/sec/men/2025.html" xr:uid="{7F9088DD-188F-344A-951A-306A0AC08E48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>